<commit_message>
add feature, don't craete new element if name is exist
</commit_message>
<xml_diff>
--- a/storage/app/data.xlsx
+++ b/storage/app/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
   <si>
     <t>Rok</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Zwierza</t>
+  </si>
+  <si>
+    <t>xXX</t>
+  </si>
+  <si>
+    <t>XXX</t>
   </si>
 </sst>
 </file>
@@ -484,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -876,6 +882,20 @@
         <v>35</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1992</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>